<commit_message>
Plantilla completada al 100%
</commit_message>
<xml_diff>
--- a/pages/plantillas/PlantillaNotas.xlsx
+++ b/pages/plantillas/PlantillaNotas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>APELLIDOS Y NOMBRES</t>
   </si>
@@ -90,12 +90,6 @@
     <t>Año Lectivo</t>
   </si>
   <si>
-    <t>Periodo</t>
-  </si>
-  <si>
-    <t>Grado</t>
-  </si>
-  <si>
     <t>Grupo</t>
   </si>
   <si>
@@ -103,6 +97,9 @@
   </si>
   <si>
     <t>Asignatura</t>
+  </si>
+  <si>
+    <t>I.H</t>
   </si>
 </sst>
 </file>
@@ -197,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -333,19 +330,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -402,9 +386,78 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -417,6 +470,9 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -426,86 +482,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -513,6 +497,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -522,12 +512,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -968,7 +952,7 @@
   <dimension ref="B2:X67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="P5" sqref="P5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,24 +974,24 @@
       <c r="B2" s="19"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="42"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="33"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="20"/>
@@ -1035,54 +1019,52 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="50"/>
+        <v>24</v>
+      </c>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38"/>
       <c r="L4" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="43"/>
+      <c r="N4" s="44"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="46"/>
-      <c r="T4" s="47"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="38"/>
     </row>
     <row r="5" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="20"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="47"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="43"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="55"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
@@ -1106,27 +1088,27 @@
       <c r="T6" s="13"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="36"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="42"/>
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
@@ -1157,11 +1139,11 @@
       <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="39"/>
+      <c r="C9" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="40"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="16" t="s">
         <v>17</v>
       </c>
@@ -1233,9 +1215,9 @@
       <c r="B11" s="22">
         <v>1</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="29"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -1262,9 +1244,9 @@
       <c r="B12" s="22">
         <v>2</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1291,9 +1273,9 @@
       <c r="B13" s="22">
         <v>3</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1320,9 +1302,9 @@
       <c r="B14" s="22">
         <v>4</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -1349,9 +1331,9 @@
       <c r="B15" s="22">
         <v>5</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1378,9 +1360,9 @@
       <c r="B16" s="22">
         <v>6</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -1407,9 +1389,9 @@
       <c r="B17" s="22">
         <v>7</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -1436,9 +1418,9 @@
       <c r="B18" s="22">
         <v>8</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -1465,9 +1447,9 @@
       <c r="B19" s="22">
         <v>9</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -1494,9 +1476,9 @@
       <c r="B20" s="22">
         <v>10</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -1523,9 +1505,9 @@
       <c r="B21" s="22">
         <v>11</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="48"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -1552,9 +1534,9 @@
       <c r="B22" s="22">
         <v>12</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="29"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="48"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -1581,9 +1563,9 @@
       <c r="B23" s="22">
         <v>13</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -1610,9 +1592,9 @@
       <c r="B24" s="22">
         <v>14</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="48"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -1639,9 +1621,9 @@
       <c r="B25" s="22">
         <v>15</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="29"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -1668,9 +1650,9 @@
       <c r="B26" s="22">
         <v>16</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="29"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -1697,9 +1679,9 @@
       <c r="B27" s="22">
         <v>17</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="29"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="48"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
@@ -1726,9 +1708,9 @@
       <c r="B28" s="22">
         <v>18</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="29"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="48"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
@@ -1755,9 +1737,9 @@
       <c r="B29" s="22">
         <v>19</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48"/>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
@@ -1784,9 +1766,9 @@
       <c r="B30" s="22">
         <v>20</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="48"/>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
@@ -1813,9 +1795,9 @@
       <c r="B31" s="22">
         <v>21</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="29"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="48"/>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -1842,9 +1824,9 @@
       <c r="B32" s="22">
         <v>22</v>
       </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="29"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="48"/>
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
@@ -1871,9 +1853,9 @@
       <c r="B33" s="22">
         <v>23</v>
       </c>
-      <c r="C33" s="27"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="29"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="48"/>
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -1900,9 +1882,9 @@
       <c r="B34" s="22">
         <v>24</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="29"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="48"/>
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
@@ -1929,9 +1911,9 @@
       <c r="B35" s="22">
         <v>25</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="29"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
@@ -1958,9 +1940,9 @@
       <c r="B36" s="22">
         <v>26</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="29"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="48"/>
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
@@ -1987,9 +1969,9 @@
       <c r="B37" s="22">
         <v>27</v>
       </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="29"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="48"/>
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
@@ -2016,9 +1998,9 @@
       <c r="B38" s="22">
         <v>28</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="29"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="48"/>
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -2045,9 +2027,9 @@
       <c r="B39" s="22">
         <v>29</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="29"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
@@ -2074,9 +2056,9 @@
       <c r="B40" s="22">
         <v>30</v>
       </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="29"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="48"/>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -2103,9 +2085,9 @@
       <c r="B41" s="22">
         <v>31</v>
       </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="29"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="48"/>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -2132,9 +2114,9 @@
       <c r="B42" s="22">
         <v>32</v>
       </c>
-      <c r="C42" s="27"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="29"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="48"/>
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
@@ -2161,9 +2143,9 @@
       <c r="B43" s="22">
         <v>33</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="48"/>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
@@ -2190,9 +2172,9 @@
       <c r="B44" s="22">
         <v>34</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="29"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="48"/>
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
@@ -2219,9 +2201,9 @@
       <c r="B45" s="22">
         <v>35</v>
       </c>
-      <c r="C45" s="27"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="48"/>
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
@@ -2248,9 +2230,9 @@
       <c r="B46" s="22">
         <v>36</v>
       </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="29"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="48"/>
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
@@ -2277,9 +2259,9 @@
       <c r="B47" s="22">
         <v>37</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="29"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
@@ -2306,9 +2288,9 @@
       <c r="B48" s="22">
         <v>38</v>
       </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="29"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="47"/>
+      <c r="E48" s="48"/>
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
@@ -2335,9 +2317,9 @@
       <c r="B49" s="22">
         <v>39</v>
       </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="29"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="48"/>
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
@@ -2364,9 +2346,9 @@
       <c r="B50" s="22">
         <v>40</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="29"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="48"/>
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
@@ -2393,9 +2375,9 @@
       <c r="B51" s="22">
         <v>41</v>
       </c>
-      <c r="C51" s="27"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="29"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="48"/>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
@@ -2422,9 +2404,9 @@
       <c r="B52" s="22">
         <v>42</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="29"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="48"/>
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
@@ -2451,9 +2433,9 @@
       <c r="B53" s="22">
         <v>43</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="48"/>
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
@@ -2480,9 +2462,9 @@
       <c r="B54" s="22">
         <v>44</v>
       </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="29"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="48"/>
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
@@ -2509,9 +2491,9 @@
       <c r="B55" s="22">
         <v>45</v>
       </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="29"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="48"/>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
@@ -2538,9 +2520,9 @@
       <c r="B56" s="22">
         <v>46</v>
       </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="29"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="48"/>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
@@ -2564,11 +2546,11 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C58" s="30" t="s">
+      <c r="C58" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="31"/>
-      <c r="E58" s="32"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="52"/>
       <c r="F58" s="3"/>
       <c r="G58" s="4">
         <f>MAX(G11:G56)</f>
@@ -2624,11 +2606,11 @@
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C59" s="30" t="s">
+      <c r="C59" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="31"/>
-      <c r="E59" s="32"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="52"/>
       <c r="F59" s="3"/>
       <c r="G59" s="4">
         <f>MIN(G11:G56)</f>
@@ -2684,158 +2666,208 @@
       </c>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C62" s="51" t="s">
+      <c r="C62" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D62" s="51"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="53"/>
-      <c r="G62" s="53"/>
-      <c r="H62" s="53"/>
-      <c r="I62" s="53"/>
-      <c r="J62" s="54"/>
-      <c r="K62" s="51" t="s">
+      <c r="D62" s="26"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="30"/>
+      <c r="K62" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="L62" s="51"/>
-      <c r="M62" s="55"/>
-      <c r="N62" s="55"/>
-      <c r="O62" s="55"/>
-      <c r="P62" s="55"/>
-      <c r="Q62" s="55"/>
-      <c r="R62" s="55"/>
-      <c r="S62" s="55"/>
+      <c r="L62" s="26"/>
+      <c r="M62" s="27"/>
+      <c r="N62" s="27"/>
+      <c r="O62" s="27"/>
+      <c r="P62" s="27"/>
+      <c r="Q62" s="27"/>
+      <c r="R62" s="27"/>
+      <c r="S62" s="27"/>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C63" s="51" t="s">
+      <c r="C63" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D63" s="51"/>
-      <c r="E63" s="52"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="54"/>
-      <c r="K63" s="51" t="s">
+      <c r="D63" s="26"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="L63" s="51"/>
-      <c r="M63" s="55"/>
-      <c r="N63" s="55"/>
-      <c r="O63" s="55"/>
-      <c r="P63" s="55"/>
-      <c r="Q63" s="55"/>
-      <c r="R63" s="55"/>
-      <c r="S63" s="55"/>
+      <c r="L63" s="26"/>
+      <c r="M63" s="27"/>
+      <c r="N63" s="27"/>
+      <c r="O63" s="27"/>
+      <c r="P63" s="27"/>
+      <c r="Q63" s="27"/>
+      <c r="R63" s="27"/>
+      <c r="S63" s="27"/>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C64" s="51" t="s">
+      <c r="C64" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="51"/>
-      <c r="E64" s="52"/>
-      <c r="F64" s="53"/>
-      <c r="G64" s="53"/>
-      <c r="H64" s="53"/>
-      <c r="I64" s="53"/>
-      <c r="J64" s="54"/>
-      <c r="K64" s="51" t="s">
+      <c r="D64" s="26"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="30"/>
+      <c r="K64" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="L64" s="51"/>
-      <c r="M64" s="55"/>
-      <c r="N64" s="55"/>
-      <c r="O64" s="55"/>
-      <c r="P64" s="55"/>
-      <c r="Q64" s="55"/>
-      <c r="R64" s="55"/>
-      <c r="S64" s="55"/>
+      <c r="L64" s="26"/>
+      <c r="M64" s="27"/>
+      <c r="N64" s="27"/>
+      <c r="O64" s="27"/>
+      <c r="P64" s="27"/>
+      <c r="Q64" s="27"/>
+      <c r="R64" s="27"/>
+      <c r="S64" s="27"/>
     </row>
     <row r="65" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C65" s="51" t="s">
+      <c r="C65" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="51"/>
-      <c r="E65" s="52"/>
-      <c r="F65" s="53"/>
-      <c r="G65" s="53"/>
-      <c r="H65" s="53"/>
-      <c r="I65" s="53"/>
-      <c r="J65" s="54"/>
-      <c r="K65" s="51" t="s">
+      <c r="D65" s="26"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="L65" s="51"/>
-      <c r="M65" s="55"/>
-      <c r="N65" s="55"/>
-      <c r="O65" s="55"/>
-      <c r="P65" s="55"/>
-      <c r="Q65" s="55"/>
-      <c r="R65" s="55"/>
-      <c r="S65" s="55"/>
+      <c r="L65" s="26"/>
+      <c r="M65" s="27"/>
+      <c r="N65" s="27"/>
+      <c r="O65" s="27"/>
+      <c r="P65" s="27"/>
+      <c r="Q65" s="27"/>
+      <c r="R65" s="27"/>
+      <c r="S65" s="27"/>
     </row>
     <row r="66" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C66" s="51" t="s">
+      <c r="C66" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="51"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="53"/>
-      <c r="G66" s="53"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="53"/>
-      <c r="J66" s="54"/>
-      <c r="K66" s="51" t="s">
+      <c r="D66" s="26"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="30"/>
+      <c r="K66" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="L66" s="51"/>
-      <c r="M66" s="55"/>
-      <c r="N66" s="55"/>
-      <c r="O66" s="55"/>
-      <c r="P66" s="55"/>
-      <c r="Q66" s="55"/>
-      <c r="R66" s="55"/>
-      <c r="S66" s="55"/>
+      <c r="L66" s="26"/>
+      <c r="M66" s="27"/>
+      <c r="N66" s="27"/>
+      <c r="O66" s="27"/>
+      <c r="P66" s="27"/>
+      <c r="Q66" s="27"/>
+      <c r="R66" s="27"/>
+      <c r="S66" s="27"/>
     </row>
     <row r="67" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C67" s="51" t="s">
+      <c r="C67" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D67" s="51"/>
-      <c r="E67" s="52"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="53"/>
-      <c r="I67" s="53"/>
-      <c r="J67" s="54"/>
-      <c r="K67" s="51" t="s">
+      <c r="D67" s="26"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="29"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="30"/>
+      <c r="K67" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L67" s="51"/>
-      <c r="M67" s="55"/>
-      <c r="N67" s="55"/>
-      <c r="O67" s="55"/>
-      <c r="P67" s="55"/>
-      <c r="Q67" s="55"/>
-      <c r="R67" s="55"/>
-      <c r="S67" s="55"/>
+      <c r="L67" s="26"/>
+      <c r="M67" s="27"/>
+      <c r="N67" s="27"/>
+      <c r="O67" s="27"/>
+      <c r="P67" s="27"/>
+      <c r="Q67" s="27"/>
+      <c r="R67" s="27"/>
+      <c r="S67" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="P7HlspHMxZBAlOJbiR6wiSrh88nxkvQdTZKJFZwr9DZ3rAOZq5F5NV0RhI0PppvfEJcw61t6/sY71tMNb70Zlw==" saltValue="8xtoVRfTFBOe7/+mmi2vTw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="IhGLUhgDvEZGpJoW1Usna5lILXqCWOsrb7G6w+vemn1gqHDtWKQIKtWeyUp5FCwGOVPBG+ggFmPXtkCqp7RE5Q==" saltValue="DT6LzFr51tORvgI5DOi8ng==" spinCount="100000" sqref="C62:S67" name="Notas Especidficaciones"/>
     <protectedRange algorithmName="SHA-512" hashValue="WbUVhdwIpZzOhLgCf/IaTr+eHaoidiAvDlVEvqqssibD2/t7cn7cMKx4vwGqZPss3wFZ6/Lm3OInbq8n2+kC+Q==" saltValue="jeXRAhwWHBaHwdR2bVFgUA==" spinCount="100000" sqref="C11:R56" name="Notas"/>
   </protectedRanges>
-  <mergeCells count="83">
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="M62:S62"/>
-    <mergeCell ref="M63:S63"/>
-    <mergeCell ref="M64:S64"/>
-    <mergeCell ref="M65:S65"/>
-    <mergeCell ref="M66:S66"/>
-    <mergeCell ref="M67:S67"/>
+  <mergeCells count="82">
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="B7:T7"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="E2:T2"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:T4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="F5:K5"/>
     <mergeCell ref="C67:D67"/>
     <mergeCell ref="K62:L62"/>
     <mergeCell ref="K63:L63"/>
@@ -2852,72 +2884,21 @@
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E2:T2"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="B7:T7"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="M62:S62"/>
+    <mergeCell ref="M63:S63"/>
+    <mergeCell ref="M64:S64"/>
+    <mergeCell ref="M65:S65"/>
+    <mergeCell ref="M66:S66"/>
+    <mergeCell ref="M67:S67"/>
   </mergeCells>
   <conditionalFormatting sqref="S11:S56">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
+      <formula>3.5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
-      <formula>3.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11:S56">
@@ -2932,12 +2913,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
-      <formula>3.0001</formula>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+      <formula>3</formula>
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
-      <formula>3</formula>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="between">
+      <formula>3.0001</formula>
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Asignar-Cambiar Alumnos Grupo 100%
</commit_message>
<xml_diff>
--- a/pages/plantillas/PlantillaNotas.xlsx
+++ b/pages/plantillas/PlantillaNotas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Calificaciones" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>APELLIDOS Y NOMBRES</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>FALTAS</t>
+  </si>
+  <si>
+    <t>Codigo Asignatura</t>
   </si>
 </sst>
 </file>
@@ -333,6 +336,57 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,21 +396,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -366,24 +405,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,24 +412,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -476,7 +479,7 @@
         <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D4FAC3-DCDF-4C71-BAC6-661695A86C3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F6D4FAC3-DCDF-4C71-BAC6-661695A86C3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -800,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Y67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58:T59"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,7 +816,9 @@
     <col min="7" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" customWidth="1"/>
     <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.42578125" customWidth="1"/>
     <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -823,25 +828,25 @@
       <c r="B2" s="16"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="29"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="46"/>
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="17"/>
@@ -881,9 +886,9 @@
       <c r="L4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="44"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="46"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="52"/>
       <c r="P4" s="30" t="s">
         <v>9</v>
       </c>
@@ -909,10 +914,12 @@
       <c r="L5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="44"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="30"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="30" t="s">
+        <v>15</v>
+      </c>
       <c r="Q5" s="31"/>
       <c r="R5" s="32"/>
       <c r="S5" s="33"/>
@@ -942,28 +949,28 @@
       <c r="U6" s="10"/>
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="37"/>
+      <c r="B7" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="49"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
@@ -995,26 +1002,26 @@
       <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
+      <c r="C9" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="48"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="35"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="37"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="49"/>
       <c r="S9" s="13" t="s">
         <v>4</v>
       </c>
@@ -1055,18 +1062,18 @@
       <c r="D11" s="39"/>
       <c r="E11" s="40"/>
       <c r="F11" s="24"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="43"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="37"/>
       <c r="S11" s="26">
         <v>0</v>
       </c>
@@ -1086,18 +1093,18 @@
       <c r="D12" s="39"/>
       <c r="E12" s="40"/>
       <c r="F12" s="24"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="43"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="37"/>
       <c r="S12" s="26">
         <v>0</v>
       </c>
@@ -1117,18 +1124,18 @@
       <c r="D13" s="39"/>
       <c r="E13" s="40"/>
       <c r="F13" s="24"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="43"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="37"/>
       <c r="S13" s="26">
         <v>0</v>
       </c>
@@ -1148,18 +1155,18 @@
       <c r="D14" s="39"/>
       <c r="E14" s="40"/>
       <c r="F14" s="24"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="43"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="37"/>
       <c r="S14" s="26">
         <v>0</v>
       </c>
@@ -1179,18 +1186,18 @@
       <c r="D15" s="39"/>
       <c r="E15" s="40"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="43"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="37"/>
       <c r="S15" s="26">
         <v>0</v>
       </c>
@@ -1210,18 +1217,18 @@
       <c r="D16" s="39"/>
       <c r="E16" s="40"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="43"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="37"/>
       <c r="S16" s="26">
         <v>0</v>
       </c>
@@ -1241,18 +1248,18 @@
       <c r="D17" s="39"/>
       <c r="E17" s="40"/>
       <c r="F17" s="24"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
-      <c r="R17" s="43"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="37"/>
       <c r="S17" s="26">
         <v>0</v>
       </c>
@@ -1272,18 +1279,18 @@
       <c r="D18" s="39"/>
       <c r="E18" s="40"/>
       <c r="F18" s="24"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="43"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="37"/>
       <c r="S18" s="26">
         <v>0</v>
       </c>
@@ -1303,18 +1310,18 @@
       <c r="D19" s="39"/>
       <c r="E19" s="40"/>
       <c r="F19" s="24"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="43"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="36"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="36"/>
+      <c r="R19" s="37"/>
       <c r="S19" s="26">
         <v>0</v>
       </c>
@@ -1334,18 +1341,18 @@
       <c r="D20" s="39"/>
       <c r="E20" s="40"/>
       <c r="F20" s="24"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="43"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="37"/>
       <c r="S20" s="26">
         <v>0</v>
       </c>
@@ -1365,18 +1372,18 @@
       <c r="D21" s="39"/>
       <c r="E21" s="40"/>
       <c r="F21" s="24"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="43"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="37"/>
       <c r="S21" s="26">
         <v>0</v>
       </c>
@@ -1396,18 +1403,18 @@
       <c r="D22" s="39"/>
       <c r="E22" s="40"/>
       <c r="F22" s="24"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="43"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="37"/>
       <c r="S22" s="26">
         <v>0</v>
       </c>
@@ -1427,18 +1434,18 @@
       <c r="D23" s="39"/>
       <c r="E23" s="40"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="43"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="37"/>
       <c r="S23" s="26">
         <v>0</v>
       </c>
@@ -1458,18 +1465,18 @@
       <c r="D24" s="39"/>
       <c r="E24" s="40"/>
       <c r="F24" s="24"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="43"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="37"/>
       <c r="S24" s="26">
         <v>0</v>
       </c>
@@ -1489,18 +1496,18 @@
       <c r="D25" s="39"/>
       <c r="E25" s="40"/>
       <c r="F25" s="24"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="43"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="36"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="37"/>
       <c r="S25" s="26">
         <v>0</v>
       </c>
@@ -1520,18 +1527,18 @@
       <c r="D26" s="39"/>
       <c r="E26" s="40"/>
       <c r="F26" s="24"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="43"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="37"/>
       <c r="S26" s="26">
         <v>0</v>
       </c>
@@ -1551,18 +1558,18 @@
       <c r="D27" s="39"/>
       <c r="E27" s="40"/>
       <c r="F27" s="24"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="43"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="37"/>
       <c r="S27" s="26">
         <v>0</v>
       </c>
@@ -1582,18 +1589,18 @@
       <c r="D28" s="39"/>
       <c r="E28" s="40"/>
       <c r="F28" s="24"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="42"/>
-      <c r="P28" s="42"/>
-      <c r="Q28" s="42"/>
-      <c r="R28" s="43"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="36"/>
+      <c r="N28" s="36"/>
+      <c r="O28" s="36"/>
+      <c r="P28" s="36"/>
+      <c r="Q28" s="36"/>
+      <c r="R28" s="37"/>
       <c r="S28" s="26">
         <v>0</v>
       </c>
@@ -1613,18 +1620,18 @@
       <c r="D29" s="39"/>
       <c r="E29" s="40"/>
       <c r="F29" s="24"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="42"/>
-      <c r="L29" s="42"/>
-      <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="42"/>
-      <c r="P29" s="42"/>
-      <c r="Q29" s="42"/>
-      <c r="R29" s="43"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+      <c r="M29" s="36"/>
+      <c r="N29" s="36"/>
+      <c r="O29" s="36"/>
+      <c r="P29" s="36"/>
+      <c r="Q29" s="36"/>
+      <c r="R29" s="37"/>
       <c r="S29" s="26">
         <v>0</v>
       </c>
@@ -1644,18 +1651,18 @@
       <c r="D30" s="39"/>
       <c r="E30" s="40"/>
       <c r="F30" s="24"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="42"/>
-      <c r="P30" s="42"/>
-      <c r="Q30" s="42"/>
-      <c r="R30" s="43"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="37"/>
       <c r="S30" s="26">
         <v>0</v>
       </c>
@@ -1675,18 +1682,18 @@
       <c r="D31" s="39"/>
       <c r="E31" s="40"/>
       <c r="F31" s="24"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="43"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="36"/>
+      <c r="O31" s="36"/>
+      <c r="P31" s="36"/>
+      <c r="Q31" s="36"/>
+      <c r="R31" s="37"/>
       <c r="S31" s="26">
         <v>0</v>
       </c>
@@ -1706,18 +1713,18 @@
       <c r="D32" s="39"/>
       <c r="E32" s="40"/>
       <c r="F32" s="24"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="43"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="36"/>
+      <c r="N32" s="36"/>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="37"/>
       <c r="S32" s="26">
         <v>0</v>
       </c>
@@ -1737,18 +1744,18 @@
       <c r="D33" s="39"/>
       <c r="E33" s="40"/>
       <c r="F33" s="24"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="43"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="37"/>
       <c r="S33" s="26">
         <v>0</v>
       </c>
@@ -1768,18 +1775,18 @@
       <c r="D34" s="39"/>
       <c r="E34" s="40"/>
       <c r="F34" s="24"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="43"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="37"/>
       <c r="S34" s="26">
         <v>0</v>
       </c>
@@ -1799,18 +1806,18 @@
       <c r="D35" s="39"/>
       <c r="E35" s="40"/>
       <c r="F35" s="24"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="42"/>
-      <c r="R35" s="43"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="36"/>
+      <c r="M35" s="36"/>
+      <c r="N35" s="36"/>
+      <c r="O35" s="36"/>
+      <c r="P35" s="36"/>
+      <c r="Q35" s="36"/>
+      <c r="R35" s="37"/>
       <c r="S35" s="26">
         <v>0</v>
       </c>
@@ -1830,18 +1837,18 @@
       <c r="D36" s="39"/>
       <c r="E36" s="40"/>
       <c r="F36" s="24"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="43"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="37"/>
       <c r="S36" s="26">
         <v>0</v>
       </c>
@@ -1861,18 +1868,18 @@
       <c r="D37" s="39"/>
       <c r="E37" s="40"/>
       <c r="F37" s="24"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="42"/>
-      <c r="L37" s="42"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="42"/>
-      <c r="P37" s="42"/>
-      <c r="Q37" s="42"/>
-      <c r="R37" s="43"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="36"/>
+      <c r="N37" s="36"/>
+      <c r="O37" s="36"/>
+      <c r="P37" s="36"/>
+      <c r="Q37" s="36"/>
+      <c r="R37" s="37"/>
       <c r="S37" s="26">
         <v>0</v>
       </c>
@@ -1892,18 +1899,18 @@
       <c r="D38" s="39"/>
       <c r="E38" s="40"/>
       <c r="F38" s="24"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42"/>
-      <c r="O38" s="42"/>
-      <c r="P38" s="42"/>
-      <c r="Q38" s="42"/>
-      <c r="R38" s="43"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36"/>
+      <c r="N38" s="36"/>
+      <c r="O38" s="36"/>
+      <c r="P38" s="36"/>
+      <c r="Q38" s="36"/>
+      <c r="R38" s="37"/>
       <c r="S38" s="26">
         <v>0</v>
       </c>
@@ -1923,18 +1930,18 @@
       <c r="D39" s="39"/>
       <c r="E39" s="40"/>
       <c r="F39" s="24"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="42"/>
-      <c r="L39" s="42"/>
-      <c r="M39" s="42"/>
-      <c r="N39" s="42"/>
-      <c r="O39" s="42"/>
-      <c r="P39" s="42"/>
-      <c r="Q39" s="42"/>
-      <c r="R39" s="43"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="36"/>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="37"/>
       <c r="S39" s="26">
         <v>0</v>
       </c>
@@ -1954,18 +1961,18 @@
       <c r="D40" s="39"/>
       <c r="E40" s="40"/>
       <c r="F40" s="24"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
-      <c r="Q40" s="42"/>
-      <c r="R40" s="43"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
+      <c r="Q40" s="36"/>
+      <c r="R40" s="37"/>
       <c r="S40" s="26">
         <v>0</v>
       </c>
@@ -1985,18 +1992,18 @@
       <c r="D41" s="39"/>
       <c r="E41" s="40"/>
       <c r="F41" s="24"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="42"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="42"/>
-      <c r="R41" s="43"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="36"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="36"/>
+      <c r="M41" s="36"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="37"/>
       <c r="S41" s="26">
         <v>0</v>
       </c>
@@ -2016,18 +2023,18 @@
       <c r="D42" s="39"/>
       <c r="E42" s="40"/>
       <c r="F42" s="24"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="42"/>
-      <c r="Q42" s="42"/>
-      <c r="R42" s="43"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="36"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
+      <c r="O42" s="36"/>
+      <c r="P42" s="36"/>
+      <c r="Q42" s="36"/>
+      <c r="R42" s="37"/>
       <c r="S42" s="26">
         <v>0</v>
       </c>
@@ -2047,18 +2054,18 @@
       <c r="D43" s="39"/>
       <c r="E43" s="40"/>
       <c r="F43" s="24"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="42"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="43"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="36"/>
+      <c r="N43" s="36"/>
+      <c r="O43" s="36"/>
+      <c r="P43" s="36"/>
+      <c r="Q43" s="36"/>
+      <c r="R43" s="37"/>
       <c r="S43" s="26">
         <v>0</v>
       </c>
@@ -2078,18 +2085,18 @@
       <c r="D44" s="39"/>
       <c r="E44" s="40"/>
       <c r="F44" s="24"/>
-      <c r="G44" s="41"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
-      <c r="K44" s="42"/>
-      <c r="L44" s="42"/>
-      <c r="M44" s="42"/>
-      <c r="N44" s="42"/>
-      <c r="O44" s="42"/>
-      <c r="P44" s="42"/>
-      <c r="Q44" s="42"/>
-      <c r="R44" s="43"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="36"/>
+      <c r="L44" s="36"/>
+      <c r="M44" s="36"/>
+      <c r="N44" s="36"/>
+      <c r="O44" s="36"/>
+      <c r="P44" s="36"/>
+      <c r="Q44" s="36"/>
+      <c r="R44" s="37"/>
       <c r="S44" s="26">
         <v>0</v>
       </c>
@@ -2109,18 +2116,18 @@
       <c r="D45" s="39"/>
       <c r="E45" s="40"/>
       <c r="F45" s="24"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="42"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="42"/>
-      <c r="N45" s="42"/>
-      <c r="O45" s="42"/>
-      <c r="P45" s="42"/>
-      <c r="Q45" s="42"/>
-      <c r="R45" s="43"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="36"/>
+      <c r="Q45" s="36"/>
+      <c r="R45" s="37"/>
       <c r="S45" s="26">
         <v>0</v>
       </c>
@@ -2140,18 +2147,18 @@
       <c r="D46" s="39"/>
       <c r="E46" s="40"/>
       <c r="F46" s="24"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="42"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="42"/>
-      <c r="O46" s="42"/>
-      <c r="P46" s="42"/>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="43"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
+      <c r="K46" s="36"/>
+      <c r="L46" s="36"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="36"/>
+      <c r="P46" s="36"/>
+      <c r="Q46" s="36"/>
+      <c r="R46" s="37"/>
       <c r="S46" s="26">
         <v>0</v>
       </c>
@@ -2171,18 +2178,18 @@
       <c r="D47" s="39"/>
       <c r="E47" s="40"/>
       <c r="F47" s="24"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="42"/>
-      <c r="L47" s="42"/>
-      <c r="M47" s="42"/>
-      <c r="N47" s="42"/>
-      <c r="O47" s="42"/>
-      <c r="P47" s="42"/>
-      <c r="Q47" s="42"/>
-      <c r="R47" s="43"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="36"/>
+      <c r="P47" s="36"/>
+      <c r="Q47" s="36"/>
+      <c r="R47" s="37"/>
       <c r="S47" s="26">
         <v>0</v>
       </c>
@@ -2202,18 +2209,18 @@
       <c r="D48" s="39"/>
       <c r="E48" s="40"/>
       <c r="F48" s="24"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
-      <c r="N48" s="42"/>
-      <c r="O48" s="42"/>
-      <c r="P48" s="42"/>
-      <c r="Q48" s="42"/>
-      <c r="R48" s="43"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="36"/>
+      <c r="O48" s="36"/>
+      <c r="P48" s="36"/>
+      <c r="Q48" s="36"/>
+      <c r="R48" s="37"/>
       <c r="S48" s="26">
         <v>0</v>
       </c>
@@ -2233,18 +2240,18 @@
       <c r="D49" s="39"/>
       <c r="E49" s="40"/>
       <c r="F49" s="24"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
-      <c r="L49" s="42"/>
-      <c r="M49" s="42"/>
-      <c r="N49" s="42"/>
-      <c r="O49" s="42"/>
-      <c r="P49" s="42"/>
-      <c r="Q49" s="42"/>
-      <c r="R49" s="43"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="36"/>
+      <c r="N49" s="36"/>
+      <c r="O49" s="36"/>
+      <c r="P49" s="36"/>
+      <c r="Q49" s="36"/>
+      <c r="R49" s="37"/>
       <c r="S49" s="26">
         <v>0</v>
       </c>
@@ -2264,18 +2271,18 @@
       <c r="D50" s="39"/>
       <c r="E50" s="40"/>
       <c r="F50" s="24"/>
-      <c r="G50" s="41"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="42"/>
-      <c r="L50" s="42"/>
-      <c r="M50" s="42"/>
-      <c r="N50" s="42"/>
-      <c r="O50" s="42"/>
-      <c r="P50" s="42"/>
-      <c r="Q50" s="42"/>
-      <c r="R50" s="43"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="36"/>
+      <c r="O50" s="36"/>
+      <c r="P50" s="36"/>
+      <c r="Q50" s="36"/>
+      <c r="R50" s="37"/>
       <c r="S50" s="26">
         <v>0</v>
       </c>
@@ -2295,18 +2302,18 @@
       <c r="D51" s="39"/>
       <c r="E51" s="40"/>
       <c r="F51" s="24"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="42"/>
-      <c r="L51" s="42"/>
-      <c r="M51" s="42"/>
-      <c r="N51" s="42"/>
-      <c r="O51" s="42"/>
-      <c r="P51" s="42"/>
-      <c r="Q51" s="42"/>
-      <c r="R51" s="43"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="36"/>
+      <c r="N51" s="36"/>
+      <c r="O51" s="36"/>
+      <c r="P51" s="36"/>
+      <c r="Q51" s="36"/>
+      <c r="R51" s="37"/>
       <c r="S51" s="26">
         <v>0</v>
       </c>
@@ -2326,18 +2333,18 @@
       <c r="D52" s="39"/>
       <c r="E52" s="40"/>
       <c r="F52" s="24"/>
-      <c r="G52" s="41"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="42"/>
-      <c r="J52" s="42"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="42"/>
-      <c r="M52" s="42"/>
-      <c r="N52" s="42"/>
-      <c r="O52" s="42"/>
-      <c r="P52" s="42"/>
-      <c r="Q52" s="42"/>
-      <c r="R52" s="43"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="36"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="36"/>
+      <c r="P52" s="36"/>
+      <c r="Q52" s="36"/>
+      <c r="R52" s="37"/>
       <c r="S52" s="26">
         <v>0</v>
       </c>
@@ -2357,18 +2364,18 @@
       <c r="D53" s="39"/>
       <c r="E53" s="40"/>
       <c r="F53" s="24"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="42"/>
-      <c r="N53" s="42"/>
-      <c r="O53" s="42"/>
-      <c r="P53" s="42"/>
-      <c r="Q53" s="42"/>
-      <c r="R53" s="43"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="36"/>
+      <c r="M53" s="36"/>
+      <c r="N53" s="36"/>
+      <c r="O53" s="36"/>
+      <c r="P53" s="36"/>
+      <c r="Q53" s="36"/>
+      <c r="R53" s="37"/>
       <c r="S53" s="26">
         <v>0</v>
       </c>
@@ -2388,18 +2395,18 @@
       <c r="D54" s="39"/>
       <c r="E54" s="40"/>
       <c r="F54" s="24"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="42"/>
-      <c r="I54" s="42"/>
-      <c r="J54" s="42"/>
-      <c r="K54" s="42"/>
-      <c r="L54" s="42"/>
-      <c r="M54" s="42"/>
-      <c r="N54" s="42"/>
-      <c r="O54" s="42"/>
-      <c r="P54" s="42"/>
-      <c r="Q54" s="42"/>
-      <c r="R54" s="43"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="36"/>
+      <c r="L54" s="36"/>
+      <c r="M54" s="36"/>
+      <c r="N54" s="36"/>
+      <c r="O54" s="36"/>
+      <c r="P54" s="36"/>
+      <c r="Q54" s="36"/>
+      <c r="R54" s="37"/>
       <c r="S54" s="26">
         <v>0</v>
       </c>
@@ -2419,18 +2426,18 @@
       <c r="D55" s="39"/>
       <c r="E55" s="40"/>
       <c r="F55" s="24"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="42"/>
-      <c r="I55" s="42"/>
-      <c r="J55" s="42"/>
-      <c r="K55" s="42"/>
-      <c r="L55" s="42"/>
-      <c r="M55" s="42"/>
-      <c r="N55" s="42"/>
-      <c r="O55" s="42"/>
-      <c r="P55" s="42"/>
-      <c r="Q55" s="42"/>
-      <c r="R55" s="43"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="36"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="36"/>
+      <c r="L55" s="36"/>
+      <c r="M55" s="36"/>
+      <c r="N55" s="36"/>
+      <c r="O55" s="36"/>
+      <c r="P55" s="36"/>
+      <c r="Q55" s="36"/>
+      <c r="R55" s="37"/>
       <c r="S55" s="26">
         <v>0</v>
       </c>
@@ -2450,18 +2457,18 @@
       <c r="D56" s="39"/>
       <c r="E56" s="40"/>
       <c r="F56" s="24"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="42"/>
-      <c r="J56" s="42"/>
-      <c r="K56" s="42"/>
-      <c r="L56" s="42"/>
-      <c r="M56" s="42"/>
-      <c r="N56" s="42"/>
-      <c r="O56" s="42"/>
-      <c r="P56" s="42"/>
-      <c r="Q56" s="42"/>
-      <c r="R56" s="43"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="36"/>
+      <c r="J56" s="36"/>
+      <c r="K56" s="36"/>
+      <c r="L56" s="36"/>
+      <c r="M56" s="36"/>
+      <c r="N56" s="36"/>
+      <c r="O56" s="36"/>
+      <c r="P56" s="36"/>
+      <c r="Q56" s="36"/>
+      <c r="R56" s="37"/>
       <c r="S56" s="26">
         <v>0</v>
       </c>
@@ -2488,24 +2495,24 @@
       <c r="R57" s="25"/>
     </row>
     <row r="58" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D58" s="48"/>
-      <c r="E58" s="49"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="43"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="50"/>
-      <c r="H58" s="51"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="51"/>
-      <c r="K58" s="51"/>
-      <c r="L58" s="51"/>
-      <c r="M58" s="51"/>
-      <c r="N58" s="51"/>
-      <c r="O58" s="51"/>
-      <c r="P58" s="51"/>
-      <c r="Q58" s="51"/>
-      <c r="R58" s="52"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="28"/>
+      <c r="I58" s="28"/>
+      <c r="J58" s="28"/>
+      <c r="K58" s="28"/>
+      <c r="L58" s="28"/>
+      <c r="M58" s="28"/>
+      <c r="N58" s="28"/>
+      <c r="O58" s="28"/>
+      <c r="P58" s="28"/>
+      <c r="Q58" s="28"/>
+      <c r="R58" s="29"/>
       <c r="S58" s="3">
         <f>MAX(S11:S56)</f>
         <v>0</v>
@@ -2516,24 +2523,24 @@
       </c>
     </row>
     <row r="59" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C59" s="47" t="s">
+      <c r="C59" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D59" s="48"/>
-      <c r="E59" s="49"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="43"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="50"/>
-      <c r="H59" s="51"/>
-      <c r="I59" s="51"/>
-      <c r="J59" s="51"/>
-      <c r="K59" s="51"/>
-      <c r="L59" s="51"/>
-      <c r="M59" s="51"/>
-      <c r="N59" s="51"/>
-      <c r="O59" s="51"/>
-      <c r="P59" s="51"/>
-      <c r="Q59" s="51"/>
-      <c r="R59" s="52"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="28"/>
+      <c r="I59" s="28"/>
+      <c r="J59" s="28"/>
+      <c r="K59" s="28"/>
+      <c r="L59" s="28"/>
+      <c r="M59" s="28"/>
+      <c r="N59" s="28"/>
+      <c r="O59" s="28"/>
+      <c r="P59" s="28"/>
+      <c r="Q59" s="28"/>
+      <c r="R59" s="29"/>
       <c r="S59" s="3">
         <f>MIN(S11:S56)</f>
         <v>0</v>
@@ -2568,11 +2575,95 @@
       <c r="B67"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NwNLlt8+VME5VC7FHz/z4xo9zHozUgOe0sa9wAK23dVRg5Mfs+Wg3pyLFOJhvktx412d+ksZpeFPcFkbdSMIVQ==" saltValue="EqSn6uS+03kb+JZyaQ+k5w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+PAbpt1nUyhyMymylAoBoHxsqxUptJcfHb4VWhLIU3c7S267DwMYRkLRiQuN1f3VAy0XCVwWX5eZfRx31jQ8lQ==" saltValue="9JBBZw4MiWzb8BVvB/AkiA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <protectedRanges>
     <protectedRange algorithmName="SHA-512" hashValue="WbUVhdwIpZzOhLgCf/IaTr+eHaoidiAvDlVEvqqssibD2/t7cn7cMKx4vwGqZPss3wFZ6/Lm3OInbq8n2+kC+Q==" saltValue="jeXRAhwWHBaHwdR2bVFgUA==" spinCount="100000" sqref="C11:R56" name="Notas"/>
   </protectedRanges>
   <mergeCells count="108">
+    <mergeCell ref="E2:U2"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="B7:U7"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="G11:R11"/>
+    <mergeCell ref="G12:R12"/>
+    <mergeCell ref="G13:R13"/>
+    <mergeCell ref="G14:R14"/>
+    <mergeCell ref="G15:R15"/>
+    <mergeCell ref="G16:R16"/>
+    <mergeCell ref="G17:R17"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="F5:K5"/>
+    <mergeCell ref="G9:R9"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="G23:R23"/>
+    <mergeCell ref="G24:R24"/>
+    <mergeCell ref="G25:R25"/>
+    <mergeCell ref="G26:R26"/>
+    <mergeCell ref="G27:R27"/>
+    <mergeCell ref="G18:R18"/>
+    <mergeCell ref="G19:R19"/>
+    <mergeCell ref="G20:R20"/>
+    <mergeCell ref="G21:R21"/>
+    <mergeCell ref="G22:R22"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="G34:R34"/>
+    <mergeCell ref="G35:R35"/>
+    <mergeCell ref="G36:R36"/>
+    <mergeCell ref="G37:R37"/>
+    <mergeCell ref="G28:R28"/>
+    <mergeCell ref="G29:R29"/>
+    <mergeCell ref="G30:R30"/>
+    <mergeCell ref="G31:R31"/>
+    <mergeCell ref="G32:R32"/>
     <mergeCell ref="G59:R59"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:U5"/>
@@ -2597,90 +2688,6 @@
     <mergeCell ref="G41:R41"/>
     <mergeCell ref="G42:R42"/>
     <mergeCell ref="G33:R33"/>
-    <mergeCell ref="G34:R34"/>
-    <mergeCell ref="G35:R35"/>
-    <mergeCell ref="G36:R36"/>
-    <mergeCell ref="G37:R37"/>
-    <mergeCell ref="G28:R28"/>
-    <mergeCell ref="G29:R29"/>
-    <mergeCell ref="G30:R30"/>
-    <mergeCell ref="G31:R31"/>
-    <mergeCell ref="G32:R32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="G23:R23"/>
-    <mergeCell ref="G24:R24"/>
-    <mergeCell ref="G25:R25"/>
-    <mergeCell ref="G26:R26"/>
-    <mergeCell ref="G27:R27"/>
-    <mergeCell ref="G18:R18"/>
-    <mergeCell ref="G19:R19"/>
-    <mergeCell ref="G20:R20"/>
-    <mergeCell ref="G21:R21"/>
-    <mergeCell ref="G22:R22"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="E2:U2"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="B7:U7"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="G11:R11"/>
-    <mergeCell ref="G12:R12"/>
-    <mergeCell ref="G13:R13"/>
-    <mergeCell ref="G14:R14"/>
-    <mergeCell ref="G15:R15"/>
-    <mergeCell ref="G16:R16"/>
-    <mergeCell ref="G17:R17"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="F5:K5"/>
-    <mergeCell ref="G9:R9"/>
   </mergeCells>
   <conditionalFormatting sqref="S11:S56">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="between">

</xml_diff>